<commit_message>
Added training review result for Ruchi ma'am
</commit_message>
<xml_diff>
--- a/Result - Training Review.xlsx
+++ b/Result - Training Review.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashn\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SNB-Personal\Projects\Qrencia 2.0\Plans\Training Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BD9FB4-6467-4692-A0EB-56CD64F49314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="21">
   <si>
     <t>Aspects</t>
   </si>
@@ -110,11 +111,14 @@
   <si>
     <t>RUCHI PAREEK</t>
   </si>
+  <si>
+    <t>NA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -221,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -246,9 +250,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -539,11 +540,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,13 +556,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
@@ -571,13 +572,13 @@
       <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -692,13 +693,13 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
@@ -812,14 +813,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
+    <row r="21" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
     </row>
     <row r="22" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
@@ -845,7 +846,9 @@
       <c r="B23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="9"/>
+      <c r="C23" s="6">
+        <v>1.5</v>
+      </c>
       <c r="D23" s="6">
         <v>1</v>
       </c>
@@ -860,7 +863,9 @@
       <c r="B24" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="9"/>
+      <c r="C24" s="6">
+        <v>1</v>
+      </c>
       <c r="D24" s="4">
         <v>2</v>
       </c>
@@ -875,7 +880,9 @@
       <c r="B25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="9"/>
+      <c r="C25" s="6">
+        <v>1.5</v>
+      </c>
       <c r="D25" s="4">
         <v>2</v>
       </c>
@@ -890,9 +897,15 @@
       <c r="B26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="2"/>
+      <c r="C26" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
@@ -901,12 +914,21 @@
       <c r="B27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="2"/>
+      <c r="C27" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C28" s="10"/>
+      <c r="C28" s="5">
+        <f>SUM(C23:C27)</f>
+        <v>4</v>
+      </c>
       <c r="D28" s="5">
         <f>SUM(D23:D27)</f>
         <v>5</v>

</xml_diff>